<commit_message>
i have put 2 in a cell
</commit_message>
<xml_diff>
--- a/my_demo_project.xlsx
+++ b/my_demo_project.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adnan Khan\Documents\GitHub\Demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E77931B-4E8E-4E7E-935D-147F87D05569}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C5EABF1-6AEB-45EC-A1A3-3A7BAC631C60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -358,7 +358,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -369,7 +369,7 @@
       </c>
       <c r="C1">
         <f ca="1">RANDBETWEEN(-10,0)</f>
-        <v>-4</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -378,7 +378,7 @@
       </c>
       <c r="C2">
         <f t="shared" ref="C2:C20" ca="1" si="0">RANDBETWEEN(-10,0)</f>
-        <v>-4</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -405,7 +405,7 @@
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>-4</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -414,7 +414,7 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>-6</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -426,7 +426,10 @@
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>-10</v>
+        <v>-6</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -435,7 +438,7 @@
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>-8</v>
+        <v>-10</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -444,7 +447,7 @@
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>-8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -453,7 +456,7 @@
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>-1</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -462,7 +465,7 @@
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
-        <v>-6</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -471,7 +474,7 @@
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="0"/>
-        <v>-5</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -480,7 +483,7 @@
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="0"/>
-        <v>-8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -489,7 +492,7 @@
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="0"/>
-        <v>-4</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -498,7 +501,7 @@
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="0"/>
-        <v>-2</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -507,7 +510,7 @@
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>-7</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -516,7 +519,7 @@
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="0"/>
-        <v>-8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -534,7 +537,7 @@
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="0"/>
-        <v>-2</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
i just types 4
xyz......
</commit_message>
<xml_diff>
--- a/my_demo_project.xlsx
+++ b/my_demo_project.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adnan Khan\Documents\GitHub\Demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{314EC3B0-2B60-45BC-908D-CDE8796A96BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B19C73ED-B98E-4152-98E5-229AF54CE160}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -358,7 +358,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -369,7 +369,7 @@
       </c>
       <c r="C1">
         <f ca="1">RANDBETWEEN(-10,0)</f>
-        <v>-5</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -378,7 +378,7 @@
       </c>
       <c r="C2">
         <f t="shared" ref="C2:C20" ca="1" si="0">RANDBETWEEN(-10,0)</f>
-        <v>-8</v>
+        <v>-7</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -387,7 +387,7 @@
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="0"/>
-        <v>-7</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -396,7 +396,7 @@
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>-4</v>
+        <v>-10</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -405,7 +405,7 @@
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>-7</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -426,7 +426,7 @@
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>-7</v>
+        <v>0</v>
       </c>
       <c r="F7">
         <v>2</v>
@@ -438,7 +438,7 @@
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="F8">
         <v>3</v>
@@ -452,6 +452,9 @@
         <f t="shared" ca="1" si="0"/>
         <v>-3</v>
       </c>
+      <c r="F9">
+        <v>4</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -459,7 +462,7 @@
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -468,7 +471,7 @@
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
-        <v>-3</v>
+        <v>-7</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -477,7 +480,7 @@
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="0"/>
-        <v>-10</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -486,7 +489,7 @@
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="0"/>
-        <v>-9</v>
+        <v>-7</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -495,7 +498,7 @@
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -504,7 +507,7 @@
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="0"/>
-        <v>-4</v>
+        <v>-10</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -513,7 +516,7 @@
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="0"/>
-        <v>-3</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -531,7 +534,7 @@
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="0"/>
-        <v>-9</v>
+        <v>-10</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -549,7 +552,7 @@
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="0"/>
-        <v>-8</v>
+        <v>-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
6 in my cell
changed something today
</commit_message>
<xml_diff>
--- a/my_demo_project.xlsx
+++ b/my_demo_project.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adnan Khan\Documents\GitHub\Demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B79584B9-F687-4779-9243-3D32BA7071F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9256917-D9CB-483C-A3D0-469F5A4A644B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -358,7 +358,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -369,7 +369,7 @@
       </c>
       <c r="C1">
         <f ca="1">RANDBETWEEN(-10,0)</f>
-        <v>-8</v>
+        <v>-7</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -378,7 +378,7 @@
       </c>
       <c r="C2">
         <f t="shared" ref="C2:C20" ca="1" si="0">RANDBETWEEN(-10,0)</f>
-        <v>-6</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -387,7 +387,7 @@
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="0"/>
-        <v>-7</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -396,7 +396,7 @@
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>-2</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -414,7 +414,7 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>-8</v>
+        <v>-1</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -426,7 +426,7 @@
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>-8</v>
+        <v>0</v>
       </c>
       <c r="F7">
         <v>2</v>
@@ -438,7 +438,7 @@
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>-9</v>
+        <v>0</v>
       </c>
       <c r="F8">
         <v>3</v>
@@ -450,7 +450,7 @@
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>-10</v>
+        <v>-9</v>
       </c>
       <c r="F9">
         <v>4</v>
@@ -462,7 +462,7 @@
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>-4</v>
+        <v>-10</v>
       </c>
       <c r="F10">
         <v>5</v>
@@ -474,7 +474,10 @@
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
-        <v>-9</v>
+        <v>-10</v>
+      </c>
+      <c r="F11">
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -483,7 +486,7 @@
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="0"/>
-        <v>-5</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -492,7 +495,7 @@
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -501,7 +504,7 @@
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="0"/>
-        <v>-9</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -510,7 +513,7 @@
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="0"/>
-        <v>-2</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -519,7 +522,7 @@
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="0"/>
-        <v>-7</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -528,7 +531,7 @@
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -537,7 +540,7 @@
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="0"/>
-        <v>-7</v>
+        <v>-10</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -546,7 +549,7 @@
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="0"/>
-        <v>-8</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -555,7 +558,7 @@
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="0"/>
-        <v>-6</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
7 in a cell
</commit_message>
<xml_diff>
--- a/my_demo_project.xlsx
+++ b/my_demo_project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adnan Khan\Documents\GitHub\Demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9256917-D9CB-483C-A3D0-469F5A4A644B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{112E3A77-11F2-43DC-9D57-FA01B0D6C04F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -357,8 +357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -369,7 +369,7 @@
       </c>
       <c r="C1">
         <f ca="1">RANDBETWEEN(-10,0)</f>
-        <v>-7</v>
+        <v>-10</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -378,7 +378,7 @@
       </c>
       <c r="C2">
         <f t="shared" ref="C2:C20" ca="1" si="0">RANDBETWEEN(-10,0)</f>
-        <v>-4</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -387,7 +387,7 @@
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="0"/>
-        <v>-1</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -396,7 +396,7 @@
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>-1</v>
+        <v>-7</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -405,7 +405,7 @@
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>-5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -414,7 +414,7 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>-1</v>
+        <v>-7</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -426,7 +426,7 @@
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>-9</v>
       </c>
       <c r="F7">
         <v>2</v>
@@ -438,7 +438,7 @@
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>-8</v>
       </c>
       <c r="F8">
         <v>3</v>
@@ -450,7 +450,7 @@
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>-9</v>
+        <v>-1</v>
       </c>
       <c r="F9">
         <v>4</v>
@@ -462,7 +462,7 @@
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>-10</v>
+        <v>-1</v>
       </c>
       <c r="F10">
         <v>5</v>
@@ -474,7 +474,7 @@
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
-        <v>-10</v>
+        <v>-9</v>
       </c>
       <c r="F11">
         <v>6</v>
@@ -486,7 +486,10 @@
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="0"/>
-        <v>-2</v>
+        <v>-1</v>
+      </c>
+      <c r="F12">
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -495,7 +498,7 @@
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="0"/>
-        <v>-6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -504,7 +507,7 @@
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="0"/>
-        <v>-4</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -513,7 +516,7 @@
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="0"/>
-        <v>-3</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -522,7 +525,7 @@
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="0"/>
-        <v>-5</v>
+        <v>-7</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -531,7 +534,7 @@
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="0"/>
-        <v>-2</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -540,7 +543,7 @@
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="0"/>
-        <v>-10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -549,7 +552,7 @@
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="0"/>
-        <v>-1</v>
+        <v>-10</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -558,7 +561,7 @@
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>